<commit_message>
add tauri to create desk app
</commit_message>
<xml_diff>
--- a/public/assets/docs/p-sds-votos.xlsx
+++ b/public/assets/docs/p-sds-votos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H-P\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EBBAECD-356B-4071-8002-31EB4E7096E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1797D3CE-5B2E-4168-937B-E28E981C2734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29550" yWindow="465" windowWidth="15270" windowHeight="7875" xr2:uid="{67FAD952-49A3-40B2-8EED-EB2E8BF0EA08}"/>
+    <workbookView xWindow="28335" yWindow="1260" windowWidth="15270" windowHeight="7875" xr2:uid="{67FAD952-49A3-40B2-8EED-EB2E8BF0EA08}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DNI</t>
   </si>
@@ -40,36 +40,6 @@
   </si>
   <si>
     <t>SECCION</t>
-  </si>
-  <si>
-    <t>JUAN</t>
-  </si>
-  <si>
-    <t>ROBERTO</t>
-  </si>
-  <si>
-    <t>MIGUEL</t>
-  </si>
-  <si>
-    <t>PEDRO</t>
-  </si>
-  <si>
-    <t>RAMIEREZ QUISPE</t>
-  </si>
-  <si>
-    <t>GONZALES PARIONA</t>
-  </si>
-  <si>
-    <t>QUISPE MEZA</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
 </sst>
 </file>
@@ -428,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A47372E-FBEB-4332-881F-E41ACB5BC440}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,74 +426,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7169</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4741</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2313</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1444</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>